<commit_message>
Complete build successful, saving changes.
(Floyd says, "Oh boy, are we gonna try something dangerous now?")
</commit_message>
<xml_diff>
--- a/Tables of Diffs.xlsx
+++ b/Tables of Diffs.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="19020" windowHeight="8835" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="19020" windowHeight="8835"/>
   </bookViews>
   <sheets>
-    <sheet name="Stage2" sheetId="4" r:id="rId1"/>
-    <sheet name="Stage4-pkgs" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Composite Listing" sheetId="5" r:id="rId1"/>
+    <sheet name="Stage2" sheetId="4" r:id="rId2"/>
+    <sheet name="Stage4-pkgs" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="177">
   <si>
     <t>java-common</t>
   </si>
@@ -410,6 +411,144 @@
   </si>
   <si>
     <t>stage4/00-install-packages/00-packages</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>zerofree</t>
+  </si>
+  <si>
+    <t>xz:xz-utils</t>
+  </si>
+  <si>
+    <t>xxd</t>
+  </si>
+  <si>
+    <t>xpdf</t>
+  </si>
+  <si>
+    <t>wpasupplicant</t>
+  </si>
+  <si>
+    <t>wireless-tools</t>
+  </si>
+  <si>
+    <t>rpi-chromium-mods</t>
+  </si>
+  <si>
+    <t>rfkill</t>
+  </si>
+  <si>
+    <t>realpath</t>
+  </si>
+  <si>
+    <t>raspberrypi-artwork</t>
+  </si>
+  <si>
+    <t>quilt</t>
+  </si>
+  <si>
+    <t>qemu-arm-static:qemu-user-static</t>
+  </si>
+  <si>
+    <t>pxz</t>
+  </si>
+  <si>
+    <t>policykit-1</t>
+  </si>
+  <si>
+    <t>omxplayer</t>
+  </si>
+  <si>
+    <t>net-tools</t>
+  </si>
+  <si>
+    <t>mkdosfs:dosfstools</t>
+  </si>
+  <si>
+    <t>gvfs</t>
+  </si>
+  <si>
+    <t>gtk2-engines</t>
+  </si>
+  <si>
+    <t>gstreamer1.0-x</t>
+  </si>
+  <si>
+    <t>gstreamer1.0-plugins-good</t>
+  </si>
+  <si>
+    <t>gstreamer1.0-plugins-base</t>
+  </si>
+  <si>
+    <t>gstreamer1.0-plugins-bad</t>
+  </si>
+  <si>
+    <t>gstreamer1.0-omx</t>
+  </si>
+  <si>
+    <t>gstreamer1.0-libav</t>
+  </si>
+  <si>
+    <t>gstreamer1.0-alsa</t>
+  </si>
+  <si>
+    <t>grep</t>
+  </si>
+  <si>
+    <t>gldriver-test</t>
+  </si>
+  <si>
+    <t>git</t>
+  </si>
+  <si>
+    <t>fonts-droid-fallback</t>
+  </si>
+  <si>
+    <t>firmware-realtek</t>
+  </si>
+  <si>
+    <t>firmware-ralink</t>
+  </si>
+  <si>
+    <t>firmware-misc-nonfree</t>
+  </si>
+  <si>
+    <t>firmware-libertas</t>
+  </si>
+  <si>
+    <t>firmware-brcm80211</t>
+  </si>
+  <si>
+    <t>firmware-atheros</t>
+  </si>
+  <si>
+    <t>dhcpcd5</t>
+  </si>
+  <si>
+    <t>desktop-base</t>
+  </si>
+  <si>
+    <t>debootstrap</t>
+  </si>
+  <si>
+    <t>chromium-browser</t>
+  </si>
+  <si>
+    <t>capsh:libcap2-bin</t>
+  </si>
+  <si>
+    <t>bsdtar</t>
+  </si>
+  <si>
+    <t>alsa-utils</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>WAS</t>
   </si>
 </sst>
 </file>
@@ -442,15 +581,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -574,19 +719,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -595,6 +822,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,6 +1142,1391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C177"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="22"/>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="23"/>
+      <c r="C34" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="22"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="22"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>28</v>
+      </c>
+      <c r="C72" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="23"/>
+      <c r="C74" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>110</v>
+      </c>
+      <c r="C77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="23"/>
+      <c r="C79" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>36</v>
+      </c>
+      <c r="C80" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>146</v>
+      </c>
+      <c r="C81" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="24"/>
+      <c r="C85" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>47</v>
+      </c>
+      <c r="C88" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>100</v>
+      </c>
+      <c r="C89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>68</v>
+      </c>
+      <c r="C91" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>86</v>
+      </c>
+      <c r="C92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="23"/>
+      <c r="C93" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>144</v>
+      </c>
+      <c r="C94" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>27</v>
+      </c>
+      <c r="C95" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>61</v>
+      </c>
+      <c r="C101" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>52</v>
+      </c>
+      <c r="C102" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>26</v>
+      </c>
+      <c r="C103" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>63</v>
+      </c>
+      <c r="C106" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="15"/>
+      <c r="C107" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="21"/>
+      <c r="C108" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="13"/>
+      <c r="C109" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>49</v>
+      </c>
+      <c r="C110" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>25</v>
+      </c>
+      <c r="C111" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>53</v>
+      </c>
+      <c r="C113" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>65</v>
+      </c>
+      <c r="C114" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>59</v>
+      </c>
+      <c r="C116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>70</v>
+      </c>
+      <c r="C118" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>57</v>
+      </c>
+      <c r="C120" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>60</v>
+      </c>
+      <c r="C121" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>51</v>
+      </c>
+      <c r="C122" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>62</v>
+      </c>
+      <c r="C125" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="15"/>
+      <c r="C126" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B127" s="13"/>
+      <c r="C127" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>48</v>
+      </c>
+      <c r="C128" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>101</v>
+      </c>
+      <c r="C131" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>64</v>
+      </c>
+      <c r="C132" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>67</v>
+      </c>
+      <c r="C133" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+      <c r="C134" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>58</v>
+      </c>
+      <c r="C135" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>54</v>
+      </c>
+      <c r="C136" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>56</v>
+      </c>
+      <c r="C138" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>143</v>
+      </c>
+      <c r="C139" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>142</v>
+      </c>
+      <c r="C140" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>141</v>
+      </c>
+      <c r="C141" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C143" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>117</v>
+      </c>
+      <c r="C144" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>50</v>
+      </c>
+      <c r="C146" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>31</v>
+      </c>
+      <c r="C147" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>140</v>
+      </c>
+      <c r="C148" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>139</v>
+      </c>
+      <c r="C149" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>138</v>
+      </c>
+      <c r="C150" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>123</v>
+      </c>
+      <c r="C151" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C153" s="16"/>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>35</v>
+      </c>
+      <c r="C154" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>69</v>
+      </c>
+      <c r="C155" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>66</v>
+      </c>
+      <c r="C156" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>32</v>
+      </c>
+      <c r="C157" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>23</v>
+      </c>
+      <c r="C158" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>82</v>
+      </c>
+      <c r="C160" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>87</v>
+      </c>
+      <c r="C161" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>85</v>
+      </c>
+      <c r="C162" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>34</v>
+      </c>
+      <c r="C163" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>95</v>
+      </c>
+      <c r="C164" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>120</v>
+      </c>
+      <c r="C165" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>111</v>
+      </c>
+      <c r="C166" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>102</v>
+      </c>
+      <c r="C167" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>137</v>
+      </c>
+      <c r="C168" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>46</v>
+      </c>
+      <c r="C169" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>136</v>
+      </c>
+      <c r="C170" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>19</v>
+      </c>
+      <c r="C171" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>43</v>
+      </c>
+      <c r="C172" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B173" t="s">
+        <v>135</v>
+      </c>
+      <c r="C173" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C174" s="14"/>
+    </row>
+    <row r="175" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C175" s="12"/>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>132</v>
+      </c>
+      <c r="C176" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>131</v>
+      </c>
+      <c r="C177" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -909,390 +2540,390 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B43" s="5"/>
+      <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1308,11 +2939,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B42" sqref="B42:B82"/>
     </sheetView>
   </sheetViews>
@@ -1323,636 +2954,636 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5" t="s">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5" t="s">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5" t="s">
+      <c r="A58" s="2"/>
+      <c r="B58" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1965,18 +3596,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1990,4 +3609,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>